<commit_message>
Xing's last Sunday commit
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/census/forms/census/census.xlsx
+++ b/odkx/app/config/tables/census/forms/census/census.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -4451,22 +4451,22 @@
     <t xml:space="preserve">49. Katika miezi 12 iliyopita, yoyote kati ya, nguruwe wako alipokea ivamektini?</t>
   </si>
   <si>
-    <t xml:space="preserve">50. Who is responsible and makes the decisions about drug treatment of [cattle]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50. Quem é o responsável e toma as decisões sobre o tratamento do [bovino] com medicamentos?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50. Ni nani anayewajibika na anayefanya uamuzi kuhusu matibabu ya dawa ya [ng’ombe]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50. Who is responsible and makes the decisions about drug treatment of [pigs]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50. Quem é o responsável e toma as decisões sobre o tratamento do [porcos] com medicamentos?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50. Ni nani anayewajibika na anayefanya uamuzi kuhusu matibabu ya dawa ya [nguruwe]</t>
+    <t xml:space="preserve">50. Who is responsible and makes the decisions about drug treatment of cattle?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50. Quem é o responsável e toma as decisões sobre o tratamento do bovino com medicamentos?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50. Ni nani anayewajibika na anayefanya uamuzi kuhusu matibabu ya dawa ya ng’ombe?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50. Who is responsible and makes the decisions about drug treatment of pigs?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50. Quem é o responsável e toma as decisões sobre o tratamento do porcos com medicamentos?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50. Ni nani anayewajibika na anayefanya uamuzi kuhusu matibabu ya dawa ya nguruwe?</t>
   </si>
   <si>
     <t xml:space="preserve">51. In the past 12 months, did you send your cattle to slaughter?</t>
@@ -4713,7 +4713,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4756,12 +4756,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4831,7 +4825,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4881,10 +4875,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4985,13 +4975,13 @@
   </sheetPr>
   <dimension ref="A1:V395"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.04"/>
@@ -10649,7 +10639,7 @@
       <selection pane="topLeft" activeCell="C182" activeCellId="0" sqref="C182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.32"/>
@@ -12989,7 +12979,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.07"/>
@@ -13041,7 +13031,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.94"/>
@@ -13140,7 +13130,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.6"/>
@@ -13412,7 +13402,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.72"/>
@@ -13997,7 +13987,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.27"/>
@@ -14045,8 +14035,8 @@
   </sheetPr>
   <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A273" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D294" activeCellId="0" sqref="D294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16783,7 +16773,7 @@
       <c r="B199" s="9" t="s">
         <v>1233</v>
       </c>
-      <c r="C199" s="12" t="s">
+      <c r="C199" s="11" t="s">
         <v>1234</v>
       </c>
       <c r="D199" s="9" t="s">
@@ -16828,7 +16818,7 @@
       <c r="B203" s="11" t="s">
         <v>1243</v>
       </c>
-      <c r="C203" s="12" t="s">
+      <c r="C203" s="11" t="s">
         <v>1244</v>
       </c>
       <c r="D203" s="3" t="s">
@@ -16842,10 +16832,10 @@
       <c r="B204" s="11" t="s">
         <v>1246</v>
       </c>
-      <c r="C204" s="13" t="s">
+      <c r="C204" s="12" t="s">
         <v>1247</v>
       </c>
-      <c r="D204" s="13" t="s">
+      <c r="D204" s="12" t="s">
         <v>1248</v>
       </c>
     </row>
@@ -16897,7 +16887,7 @@
       <c r="B208" s="9" t="s">
         <v>1259</v>
       </c>
-      <c r="C208" s="12" t="s">
+      <c r="C208" s="11" t="s">
         <v>1260</v>
       </c>
       <c r="D208" s="3" t="s">
@@ -18022,7 +18012,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="9" t="s">
         <v>290</v>
       </c>
@@ -18036,7 +18026,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="9" t="s">
         <v>354</v>
       </c>

</xml_diff>